<commit_message>
Regenerated charts for textual patterns in issue refactoring documentation.
</commit_message>
<xml_diff>
--- a/Python/IssueRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A1493B-30F6-483F-A850-CCB1D027C457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08791B62-87FA-449A-8FD6-6807DF4CD986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Textual_patterns_issue_titles" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="textual_patterns_treemap" sheetId="4" r:id="rId3"/>
+    <sheet name="textual_patterns_treemap" sheetId="4" r:id="rId1"/>
+    <sheet name="sunburst" sheetId="5" r:id="rId2"/>
+    <sheet name="pie_chart" sheetId="6" r:id="rId3"/>
     <sheet name="issue_title_refactoring_doc_tex" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -25,10 +25,6 @@
     <definedName name="_xlchart.v1.3" hidden="1">issue_title_refactoring_doc_tex!$A$2:$AJ$2</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">issue_title_refactoring_doc_tex!$A$1:$AJ$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">issue_title_refactoring_doc_tex!$A$2:$AJ$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">issue_title_refactoring_doc_tex!$A$1:$AJ$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">issue_title_refactoring_doc_tex!$A$2:$AJ$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">issue_title_refactoring_doc_tex!$A$1:$AJ$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">issue_title_refactoring_doc_tex!$A$2:$AJ$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -732,80 +728,15 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="2"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Proportion of Various</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Refactoring Documentation Patterns</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -813,1351 +744,58 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredPieSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:dPt>
-                  <c:idx val="0"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000001-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="1"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000003-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="2"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000005-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="3"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000007-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="4"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000009-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="5"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000000B-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="6"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000000D-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="7"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000000F-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="8"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000011-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="9"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000013-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="10"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000015-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="11"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000017-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="12"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000019-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="13"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000001B-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="14"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000001D-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="15"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000001F-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="16"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000021-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="17"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000023-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="18"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000025-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="19"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000027-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="20"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000029-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="21"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000002B-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="22"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000002D-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="23"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="80000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000002F-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="24"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000031-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="25"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000033-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="26"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000035-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="27"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000037-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="28"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000039-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="29"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000003B-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="30"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000003D-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="31"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{0000003F-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="32"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000041-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="33"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000043-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dPt>
-                  <c:idx val="34"/>
-                  <c:bubble3D val="0"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="20000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:extLst>
-                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                      <c16:uniqueId val="{00000045-0A93-425B-9B5E-096C6D2C6E06}"/>
-                    </c:ext>
-                  </c:extLst>
-                </c:dPt>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:pattFill prst="pct75">
-                      <a:fgClr>
-                        <a:sysClr val="windowText" lastClr="000000">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:sysClr>
-                      </a:fgClr>
-                      <a:bgClr>
-                        <a:sysClr val="windowText" lastClr="000000">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:sysClr>
-                      </a:bgClr>
-                    </a:pattFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                        <a:prstClr val="black">
-                          <a:alpha val="40000"/>
-                        </a:prstClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="lt1"/>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="bestFit"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="0"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="1"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                        <a:prstGeom prst="wedgeRectCallout">
-                          <a:avLst/>
-                        </a:prstGeom>
-                        <a:pattFill prst="pct75">
-                          <a:fgClr>
-                            <a:schemeClr val="dk1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:fgClr>
-                          <a:bgClr>
-                            <a:schemeClr val="dk1">
-                              <a:lumMod val="65000"/>
-                              <a:lumOff val="35000"/>
-                            </a:schemeClr>
-                          </a:bgClr>
-                        </a:pattFill>
-                        <a:ln>
-                          <a:noFill/>
-                        </a:ln>
-                      </c15:spPr>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>issue_title_refactoring_doc_tex!$A$1:$AI$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="35"/>
-                      <c:pt idx="0">
-                        <c:v>REFACTOR</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>RECODE</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>REENGINEER</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>REWRIT</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>EDIT</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>ADD</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>CHANG</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>CREAT</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>EXTEND</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>EXTRACT</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>FIX</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>IMPROV</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>INLIN</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>INTRODUC</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>MERG</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>MOV</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>REPACKAG</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>REDESIGN</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>REDUC</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>REFIN</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>REMOV</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>RENAM</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>REORGANIZ</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>REPLAC</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>RESTRUCTUR</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>SPLIT</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>CHANGTHENAME</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>CLEANUPCODE</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>CLEANUP</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>CODECLEAN</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>CODEOPTIMIZATION</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>FIXCODESTYLE</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>IMPROVCODEQUALITY</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>PULLUP</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>PUSHDOWN</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>issue_title_refactoring_doc_tex!$A$2:$AI$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="35"/>
-                      <c:pt idx="0">
-                        <c:v>4.0245566166439204</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>6.8212824010913997E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2.2737608003637999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>4.5475216007275998E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>2.34197362437471</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.38653933606184598</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>24.6930422919508</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8.0036380172805792</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>10.0727603456116</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>3.20600272851296</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>3.20600272851296</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>6.0482037289677102</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>7.0941336971350601</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.52296498408367398</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2.06912232833105</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>2.1373351523419699</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>3.56980445657116</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>2.2737608003637999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>0.20463847203274199</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>2.2737608003637999</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>0.31832651205093199</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>10.004547521600699</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>2.16007276034561</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>0.11368804001819</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>3.4333788085493402</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>1.5916325602546599</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>4.5475216007275998E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>6.8212824010913997E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>1.1368804001819</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>0.20463847203274199</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>2.2737608003637999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>9.0950432014551996E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>4.5475216007275998E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>0.15916325602546599</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>0.45475216007275998</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000046-0A93-425B-9B5E-096C6D2C6E06}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredPieSeries>
-          </c:ext>
-        </c:extLst>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
+        <c:gapWidth val="150"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -2237,15 +875,1454 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pie Chart Showing Issue Refactoring Documentation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Patterns</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="30"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="31"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="35"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-7CC1-4738-8497-CDEF205ECBE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>issue_title_refactoring_doc_tex!$A$1:$AJ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>REFACTOR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RECODE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>REENGINEER</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>REWRIT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EDIT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ADD</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CHANG</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CREAT</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>EXTEND</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EXTRACT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FIX</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>IMPROV</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>INLIN</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>INTRODUC</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MERG</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MOV</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>REPACKAG</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>REDESIGN</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>REDUC</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>REFIN</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>REMOV</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>RENAM</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>REORGANIZ</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>REPLAC</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>RESTRUCTUR</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SPLIT</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>CHANGTHENAME</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>CLEANUPCODE</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>CLEANUP</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>CODECLEAN</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>CODEOPTIMIZATION</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>FIXCODESTYLE</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>IMPROVCODEQUALITY</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>PULLUP</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>PUSHDOWN</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>SIMPLIFYCODE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>issue_title_refactoring_doc_tex!$A$2:$AJ$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>4.2531120331950198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1867219917012403E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1867219917012403E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4578146611341599E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.57607192254495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34578146611341598</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.691562932226802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.5207468879667996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6300138312586405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2157676348547701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0601659751037298</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2932226832641698</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7254495159059404</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50138312586445299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7807745504840899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.23029045643153</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6998616874135499</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.72890733056708E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.17289073305670799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.2994467496542099</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36307053941908701</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.8374827109266896</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0401106500691499</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.6445366528353995E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.5269709543568402</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.60788381742738</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.1867219917012403E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.9156293222683199E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.22752420470262</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.22475795297372</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.72890733056708E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.103734439834024</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.4578146611341599E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.121023513139695</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.414937759336099</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.121023513139695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000048-7CC1-4738-8497-CDEF205ECBE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2288,6 +2365,61 @@
           <cx:layoutPr>
             <cx:parentLabelLayout val="overlapping"/>
           </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Sunburst Showing Proportions of Textual Patterns in Issue Refactoring Documentation</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Sunburst Showing Proportions of Textual Patterns in Issue Refactoring Documentation</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{E9EDBB10-6881-4B4F-9099-8D9C6CCC3679}">
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
         </cx:series>
       </cx:plotAreaRegion>
     </cx:plotArea>
@@ -2375,8 +2507,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="411">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2387,7 +2559,19 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2410,7 +2594,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="900"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -2449,7 +2633,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2458,30 +2642,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -2491,29 +2652,15 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -2531,13 +2678,11 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -2553,13 +2698,14 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -2572,11 +2718,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -2593,10 +2737,13 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -2610,7 +2757,7 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2632,13 +2779,13 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -2688,12 +2835,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -2757,12 +2904,14 @@
                 <a:lumMod val="95000"/>
                 <a:lumOff val="5000"/>
                 <a:alpha val="42000"/>
+                <a:lumOff val="10000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
               <a:schemeClr val="lt1">
                 <a:lumMod val="75000"/>
                 <a:alpha val="36000"/>
+                <a:lumOff val="10000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -2798,13 +2947,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2826,7 +2976,7 @@
         </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:legend>
   <cs:plotArea>
     <cs:lnRef idx="0"/>
@@ -2855,7 +3005,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
@@ -2865,7 +3015,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -2875,11 +3025,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="bg1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2896,12 +3045,10 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1800" b="1"/>
   </cs:title>
   <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2912,6 +3059,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2925,7 +3073,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -2958,12 +3106,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -2977,7 +3120,517 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="411">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2988,19 +3641,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1">
-          <a:lumMod val="65000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3023,7 +3664,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -3062,7 +3703,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -3071,7 +3712,30 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -3081,15 +3745,29 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -3107,11 +3785,13 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -3127,14 +3807,13 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -3147,9 +3826,11 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -3166,13 +3847,10 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -3186,7 +3864,7 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3208,13 +3886,13 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -3264,12 +3942,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -3333,14 +4011,12 @@
                 <a:lumMod val="95000"/>
                 <a:lumOff val="5000"/>
                 <a:alpha val="42000"/>
-                <a:lumOff val="10000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
               <a:schemeClr val="lt1">
                 <a:lumMod val="75000"/>
                 <a:alpha val="36000"/>
-                <a:lumOff val="10000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -3376,14 +4052,13 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3405,7 +4080,7 @@
         </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea>
     <cs:lnRef idx="0"/>
@@ -3434,7 +4109,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
@@ -3444,7 +4119,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -3454,10 +4129,11 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="bg1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3474,10 +4150,12 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -3488,7 +4166,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3502,7 +4179,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -3535,7 +4212,12 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -3549,10 +4231,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9B3C7862-89B7-41BF-A820-69602BA42E30}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3560,10 +4242,21 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9B3C7862-89B7-41BF-A820-69602BA42E30}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A94BE6DD-BE22-4113-8C57-03C45CB641F6}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{DCA05FE5-1CE1-437F-ACEC-5315015F92F2}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3571,39 +4264,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8666922" cy="6255026"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E7D69F7-8DC8-7F7F-2AB6-218719295A72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -3657,7 +4317,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -3673,7 +4333,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F144A2-5973-C3B7-CE6B-5366EC82D7F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B829CF-2146-DC32-988F-897DFFE64966}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -3712,6 +4372,150 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8660780" cy="6253976"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D28694-DC45-928A-9F9D-C21DEA2E0BFC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C106C844-8B41-A1FF-5BAF-E565F3D7A132}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr>
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noTextEdit="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="8660780" cy="6253976"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstClr val="white"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="1">
+          <a:solidFill>
+            <a:prstClr val="green"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8660780" cy="6253976"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{451AAE07-785B-31BE-07FA-015CF8C9D4EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4010,24 +4814,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCE3BE0-2747-41DD-B68D-1164E24A2705}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
       <selection sqref="A1:AJ2"/>
     </sheetView>
   </sheetViews>
@@ -4148,112 +4938,112 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>4.0245566166439204</v>
+        <v>4.2531120331950198</v>
       </c>
       <c r="B2">
-        <v>6.8212824010913997E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="C2">
-        <v>2.2737608003637999E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="D2">
-        <v>4.5475216007275998E-2</v>
+        <v>3.4578146611341599E-2</v>
       </c>
       <c r="E2">
-        <v>2.34197362437471</v>
+        <v>2.57607192254495</v>
       </c>
       <c r="F2">
-        <v>0.38653933606184598</v>
+        <v>0.34578146611341598</v>
       </c>
       <c r="G2">
-        <v>24.6930422919508</v>
+        <v>25.691562932226802</v>
       </c>
       <c r="H2">
-        <v>8.0036380172805792</v>
+        <v>7.5207468879667996</v>
       </c>
       <c r="I2">
-        <v>10.0727603456116</v>
+        <v>9.6300138312586405</v>
       </c>
       <c r="J2">
-        <v>3.20600272851296</v>
+        <v>3.2157676348547701</v>
       </c>
       <c r="K2">
-        <v>3.20600272851296</v>
+        <v>3.0601659751037298</v>
       </c>
       <c r="L2">
-        <v>6.0482037289677102</v>
+        <v>6.2932226832641698</v>
       </c>
       <c r="M2">
-        <v>7.0941336971350601</v>
+        <v>6.7254495159059404</v>
       </c>
       <c r="N2">
-        <v>0.52296498408367398</v>
+        <v>0.50138312586445299</v>
       </c>
       <c r="O2">
-        <v>2.06912232833105</v>
+        <v>1.7807745504840899</v>
       </c>
       <c r="P2">
-        <v>2.1373351523419699</v>
+        <v>2.23029045643153</v>
       </c>
       <c r="Q2">
-        <v>3.56980445657116</v>
+        <v>3.6998616874135499</v>
       </c>
       <c r="R2">
-        <v>2.2737608003637999E-2</v>
+        <v>1.72890733056708E-2</v>
       </c>
       <c r="S2">
-        <v>0.20463847203274199</v>
+        <v>0.17289073305670799</v>
       </c>
       <c r="T2">
-        <v>2.2737608003637999</v>
+        <v>2.2994467496542099</v>
       </c>
       <c r="U2">
-        <v>0.31832651205093199</v>
+        <v>0.36307053941908701</v>
       </c>
       <c r="V2">
-        <v>10.004547521600699</v>
+        <v>9.8374827109266896</v>
       </c>
       <c r="W2">
-        <v>2.16007276034561</v>
+        <v>2.0401106500691499</v>
       </c>
       <c r="X2">
-        <v>0.11368804001819</v>
+        <v>8.6445366528353995E-2</v>
       </c>
       <c r="Y2">
-        <v>3.4333788085493402</v>
+        <v>3.5269709543568402</v>
       </c>
       <c r="Z2">
-        <v>1.5916325602546599</v>
+        <v>1.60788381742738</v>
       </c>
       <c r="AA2">
-        <v>4.5475216007275998E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="AB2">
-        <v>6.8212824010913997E-2</v>
+        <v>6.9156293222683199E-2</v>
       </c>
       <c r="AC2">
-        <v>1.1368804001819</v>
+        <v>1.22752420470262</v>
       </c>
       <c r="AD2">
-        <v>0.20463847203274199</v>
+        <v>0.22475795297372</v>
       </c>
       <c r="AE2">
-        <v>2.2737608003637999E-2</v>
+        <v>1.72890733056708E-2</v>
       </c>
       <c r="AF2">
-        <v>9.0950432014551996E-2</v>
+        <v>0.103734439834024</v>
       </c>
       <c r="AG2">
-        <v>4.5475216007275998E-2</v>
+        <v>3.4578146611341599E-2</v>
       </c>
       <c r="AH2">
-        <v>0.15916325602546599</v>
+        <v>0.121023513139695</v>
       </c>
       <c r="AI2">
-        <v>0.45475216007275998</v>
+        <v>0.414937759336099</v>
       </c>
       <c r="AJ2">
-        <v>0.13642564802182799</v>
+        <v>0.121023513139695</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
@@ -4370,112 +5160,112 @@
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" cm="1">
         <f t="array" ref="A5:AJ5">A2:AJ2</f>
-        <v>4.0245566166439204</v>
+        <v>4.2531120331950198</v>
       </c>
       <c r="B5">
-        <v>6.8212824010913997E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="C5">
-        <v>2.2737608003637999E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="D5">
-        <v>4.5475216007275998E-2</v>
+        <v>3.4578146611341599E-2</v>
       </c>
       <c r="E5">
-        <v>2.34197362437471</v>
+        <v>2.57607192254495</v>
       </c>
       <c r="F5">
-        <v>0.38653933606184598</v>
+        <v>0.34578146611341598</v>
       </c>
       <c r="G5">
-        <v>24.6930422919508</v>
+        <v>25.691562932226802</v>
       </c>
       <c r="H5">
-        <v>8.0036380172805792</v>
+        <v>7.5207468879667996</v>
       </c>
       <c r="I5">
-        <v>10.0727603456116</v>
+        <v>9.6300138312586405</v>
       </c>
       <c r="J5">
-        <v>3.20600272851296</v>
+        <v>3.2157676348547701</v>
       </c>
       <c r="K5">
-        <v>3.20600272851296</v>
+        <v>3.0601659751037298</v>
       </c>
       <c r="L5">
-        <v>6.0482037289677102</v>
+        <v>6.2932226832641698</v>
       </c>
       <c r="M5">
-        <v>7.0941336971350601</v>
+        <v>6.7254495159059404</v>
       </c>
       <c r="N5">
-        <v>0.52296498408367398</v>
+        <v>0.50138312586445299</v>
       </c>
       <c r="O5">
-        <v>2.06912232833105</v>
+        <v>1.7807745504840899</v>
       </c>
       <c r="P5">
-        <v>2.1373351523419699</v>
+        <v>2.23029045643153</v>
       </c>
       <c r="Q5">
-        <v>3.56980445657116</v>
+        <v>3.6998616874135499</v>
       </c>
       <c r="R5">
-        <v>2.2737608003637999E-2</v>
+        <v>1.72890733056708E-2</v>
       </c>
       <c r="S5">
-        <v>0.20463847203274199</v>
+        <v>0.17289073305670799</v>
       </c>
       <c r="T5">
-        <v>2.2737608003637999</v>
+        <v>2.2994467496542099</v>
       </c>
       <c r="U5">
-        <v>0.31832651205093199</v>
+        <v>0.36307053941908701</v>
       </c>
       <c r="V5">
-        <v>10.004547521600699</v>
+        <v>9.8374827109266896</v>
       </c>
       <c r="W5">
-        <v>2.16007276034561</v>
+        <v>2.0401106500691499</v>
       </c>
       <c r="X5">
-        <v>0.11368804001819</v>
+        <v>8.6445366528353995E-2</v>
       </c>
       <c r="Y5">
-        <v>3.4333788085493402</v>
+        <v>3.5269709543568402</v>
       </c>
       <c r="Z5">
-        <v>1.5916325602546599</v>
+        <v>1.60788381742738</v>
       </c>
       <c r="AA5">
-        <v>4.5475216007275998E-2</v>
+        <v>5.1867219917012403E-2</v>
       </c>
       <c r="AB5">
-        <v>6.8212824010913997E-2</v>
+        <v>6.9156293222683199E-2</v>
       </c>
       <c r="AC5">
-        <v>1.1368804001819</v>
+        <v>1.22752420470262</v>
       </c>
       <c r="AD5">
-        <v>0.20463847203274199</v>
+        <v>0.22475795297372</v>
       </c>
       <c r="AE5">
-        <v>2.2737608003637999E-2</v>
+        <v>1.72890733056708E-2</v>
       </c>
       <c r="AF5">
-        <v>9.0950432014551996E-2</v>
+        <v>0.103734439834024</v>
       </c>
       <c r="AG5">
-        <v>4.5475216007275998E-2</v>
+        <v>3.4578146611341599E-2</v>
       </c>
       <c r="AH5">
-        <v>0.15916325602546599</v>
+        <v>0.121023513139695</v>
       </c>
       <c r="AI5">
-        <v>0.45475216007275998</v>
+        <v>0.414937759336099</v>
       </c>
       <c r="AJ5">
-        <v>0.13642564802182799</v>
+        <v>0.121023513139695</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Regenerated the results for issue refactoring documentation patterns including the word cloud.
</commit_message>
<xml_diff>
--- a/Python/IssueRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08791B62-87FA-449A-8FD6-6807DF4CD986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BA918B-BC87-4017-AE38-A734CC17A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2087,112 +2087,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>4.2531120331950198</c:v>
+                  <c:v>4.2847270214236302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1867219917012403E-2</c:v>
+                  <c:v>5.1831375259156799E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1867219917012403E-2</c:v>
+                  <c:v>5.1831375259156799E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4578146611341599E-2</c:v>
+                  <c:v>3.4554250172771202E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.57607192254495</c:v>
+                  <c:v>2.57429163787145</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34578146611341598</c:v>
+                  <c:v>0.345542501727712</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.691562932226802</c:v>
+                  <c:v>25.673807878369001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5207468879667996</c:v>
+                  <c:v>7.51554941257774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.6300138312586405</c:v>
+                  <c:v>9.6233586731167904</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2157676348547701</c:v>
+                  <c:v>3.2135452660677202</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0601659751037298</c:v>
+                  <c:v>3.0580511402902499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.2932226832641698</c:v>
+                  <c:v>6.2888735314443602</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.7254495159059404</c:v>
+                  <c:v>6.7380787836903897</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.50138312586445299</c:v>
+                  <c:v>0.50103662750518296</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7807745504840899</c:v>
+                  <c:v>1.77954388389771</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.23029045643153</c:v>
+                  <c:v>2.2287491361437399</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.6998616874135499</c:v>
+                  <c:v>3.6973047684865201</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.72890733056708E-2</c:v>
+                  <c:v>1.7277125086385601E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.17289073305670799</c:v>
+                  <c:v>0.172771250863856</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2994467496542099</c:v>
+                  <c:v>2.29785763648928</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.36307053941908701</c:v>
+                  <c:v>0.36281962681409802</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.8374827109266896</c:v>
+                  <c:v>9.8479612992398007</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0401106500691499</c:v>
+                  <c:v>2.0387007601935001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.6445366528353995E-2</c:v>
+                  <c:v>8.6385625431928098E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.5269709543568402</c:v>
+                  <c:v>3.5245335176226602</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.60788381742738</c:v>
+                  <c:v>1.6067726330338601</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.1867219917012403E-2</c:v>
+                  <c:v>5.1831375259156799E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.9156293222683199E-2</c:v>
+                  <c:v>6.9108500345542501E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.22752420470262</c:v>
+                  <c:v>1.22667588113337</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.22475795297372</c:v>
+                  <c:v>0.22460262612301299</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.72890733056708E-2</c:v>
+                  <c:v>1.7277125086385601E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.103734439834024</c:v>
+                  <c:v>0.103662750518313</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.4578146611341599E-2</c:v>
+                  <c:v>3.4554250172771202E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.121023513139695</c:v>
+                  <c:v>0.120939875604699</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.414937759336099</c:v>
+                  <c:v>0.414651002073255</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.121023513139695</c:v>
+                  <c:v>0.120939875604699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4333,7 +4333,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B829CF-2146-DC32-988F-897DFFE64966}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83335651-3332-AC6B-6697-225D89E9BEEC}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -4444,7 +4444,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C106C844-8B41-A1FF-5BAF-E565F3D7A132}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{475D9659-1AF2-BA83-E201-BCE3161CA527}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -4817,7 +4817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
       <selection sqref="A1:AJ2"/>
     </sheetView>
   </sheetViews>
@@ -4938,112 +4938,112 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>4.2531120331950198</v>
+        <v>4.2847270214236302</v>
       </c>
       <c r="B2">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="C2">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="D2">
-        <v>3.4578146611341599E-2</v>
+        <v>3.4554250172771202E-2</v>
       </c>
       <c r="E2">
-        <v>2.57607192254495</v>
+        <v>2.57429163787145</v>
       </c>
       <c r="F2">
-        <v>0.34578146611341598</v>
+        <v>0.345542501727712</v>
       </c>
       <c r="G2">
-        <v>25.691562932226802</v>
+        <v>25.673807878369001</v>
       </c>
       <c r="H2">
-        <v>7.5207468879667996</v>
+        <v>7.51554941257774</v>
       </c>
       <c r="I2">
-        <v>9.6300138312586405</v>
+        <v>9.6233586731167904</v>
       </c>
       <c r="J2">
-        <v>3.2157676348547701</v>
+        <v>3.2135452660677202</v>
       </c>
       <c r="K2">
-        <v>3.0601659751037298</v>
+        <v>3.0580511402902499</v>
       </c>
       <c r="L2">
-        <v>6.2932226832641698</v>
+        <v>6.2888735314443602</v>
       </c>
       <c r="M2">
-        <v>6.7254495159059404</v>
+        <v>6.7380787836903897</v>
       </c>
       <c r="N2">
-        <v>0.50138312586445299</v>
+        <v>0.50103662750518296</v>
       </c>
       <c r="O2">
-        <v>1.7807745504840899</v>
+        <v>1.77954388389771</v>
       </c>
       <c r="P2">
-        <v>2.23029045643153</v>
+        <v>2.2287491361437399</v>
       </c>
       <c r="Q2">
-        <v>3.6998616874135499</v>
+        <v>3.6973047684865201</v>
       </c>
       <c r="R2">
-        <v>1.72890733056708E-2</v>
+        <v>1.7277125086385601E-2</v>
       </c>
       <c r="S2">
-        <v>0.17289073305670799</v>
+        <v>0.172771250863856</v>
       </c>
       <c r="T2">
-        <v>2.2994467496542099</v>
+        <v>2.29785763648928</v>
       </c>
       <c r="U2">
-        <v>0.36307053941908701</v>
+        <v>0.36281962681409802</v>
       </c>
       <c r="V2">
-        <v>9.8374827109266896</v>
+        <v>9.8479612992398007</v>
       </c>
       <c r="W2">
-        <v>2.0401106500691499</v>
+        <v>2.0387007601935001</v>
       </c>
       <c r="X2">
-        <v>8.6445366528353995E-2</v>
+        <v>8.6385625431928098E-2</v>
       </c>
       <c r="Y2">
-        <v>3.5269709543568402</v>
+        <v>3.5245335176226602</v>
       </c>
       <c r="Z2">
-        <v>1.60788381742738</v>
+        <v>1.6067726330338601</v>
       </c>
       <c r="AA2">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="AB2">
-        <v>6.9156293222683199E-2</v>
+        <v>6.9108500345542501E-2</v>
       </c>
       <c r="AC2">
-        <v>1.22752420470262</v>
+        <v>1.22667588113337</v>
       </c>
       <c r="AD2">
-        <v>0.22475795297372</v>
+        <v>0.22460262612301299</v>
       </c>
       <c r="AE2">
-        <v>1.72890733056708E-2</v>
+        <v>1.7277125086385601E-2</v>
       </c>
       <c r="AF2">
-        <v>0.103734439834024</v>
+        <v>0.103662750518313</v>
       </c>
       <c r="AG2">
-        <v>3.4578146611341599E-2</v>
+        <v>3.4554250172771202E-2</v>
       </c>
       <c r="AH2">
-        <v>0.121023513139695</v>
+        <v>0.120939875604699</v>
       </c>
       <c r="AI2">
-        <v>0.414937759336099</v>
+        <v>0.414651002073255</v>
       </c>
       <c r="AJ2">
-        <v>0.121023513139695</v>
+        <v>0.120939875604699</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
@@ -5160,112 +5160,112 @@
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" cm="1">
         <f t="array" ref="A5:AJ5">A2:AJ2</f>
-        <v>4.2531120331950198</v>
+        <v>4.2847270214236302</v>
       </c>
       <c r="B5">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="C5">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="D5">
-        <v>3.4578146611341599E-2</v>
+        <v>3.4554250172771202E-2</v>
       </c>
       <c r="E5">
-        <v>2.57607192254495</v>
+        <v>2.57429163787145</v>
       </c>
       <c r="F5">
-        <v>0.34578146611341598</v>
+        <v>0.345542501727712</v>
       </c>
       <c r="G5">
-        <v>25.691562932226802</v>
+        <v>25.673807878369001</v>
       </c>
       <c r="H5">
-        <v>7.5207468879667996</v>
+        <v>7.51554941257774</v>
       </c>
       <c r="I5">
-        <v>9.6300138312586405</v>
+        <v>9.6233586731167904</v>
       </c>
       <c r="J5">
-        <v>3.2157676348547701</v>
+        <v>3.2135452660677202</v>
       </c>
       <c r="K5">
-        <v>3.0601659751037298</v>
+        <v>3.0580511402902499</v>
       </c>
       <c r="L5">
-        <v>6.2932226832641698</v>
+        <v>6.2888735314443602</v>
       </c>
       <c r="M5">
-        <v>6.7254495159059404</v>
+        <v>6.7380787836903897</v>
       </c>
       <c r="N5">
-        <v>0.50138312586445299</v>
+        <v>0.50103662750518296</v>
       </c>
       <c r="O5">
-        <v>1.7807745504840899</v>
+        <v>1.77954388389771</v>
       </c>
       <c r="P5">
-        <v>2.23029045643153</v>
+        <v>2.2287491361437399</v>
       </c>
       <c r="Q5">
-        <v>3.6998616874135499</v>
+        <v>3.6973047684865201</v>
       </c>
       <c r="R5">
-        <v>1.72890733056708E-2</v>
+        <v>1.7277125086385601E-2</v>
       </c>
       <c r="S5">
-        <v>0.17289073305670799</v>
+        <v>0.172771250863856</v>
       </c>
       <c r="T5">
-        <v>2.2994467496542099</v>
+        <v>2.29785763648928</v>
       </c>
       <c r="U5">
-        <v>0.36307053941908701</v>
+        <v>0.36281962681409802</v>
       </c>
       <c r="V5">
-        <v>9.8374827109266896</v>
+        <v>9.8479612992398007</v>
       </c>
       <c r="W5">
-        <v>2.0401106500691499</v>
+        <v>2.0387007601935001</v>
       </c>
       <c r="X5">
-        <v>8.6445366528353995E-2</v>
+        <v>8.6385625431928098E-2</v>
       </c>
       <c r="Y5">
-        <v>3.5269709543568402</v>
+        <v>3.5245335176226602</v>
       </c>
       <c r="Z5">
-        <v>1.60788381742738</v>
+        <v>1.6067726330338601</v>
       </c>
       <c r="AA5">
-        <v>5.1867219917012403E-2</v>
+        <v>5.1831375259156799E-2</v>
       </c>
       <c r="AB5">
-        <v>6.9156293222683199E-2</v>
+        <v>6.9108500345542501E-2</v>
       </c>
       <c r="AC5">
-        <v>1.22752420470262</v>
+        <v>1.22667588113337</v>
       </c>
       <c r="AD5">
-        <v>0.22475795297372</v>
+        <v>0.22460262612301299</v>
       </c>
       <c r="AE5">
-        <v>1.72890733056708E-2</v>
+        <v>1.7277125086385601E-2</v>
       </c>
       <c r="AF5">
-        <v>0.103734439834024</v>
+        <v>0.103662750518313</v>
       </c>
       <c r="AG5">
-        <v>3.4578146611341599E-2</v>
+        <v>3.4554250172771202E-2</v>
       </c>
       <c r="AH5">
-        <v>0.121023513139695</v>
+        <v>0.120939875604699</v>
       </c>
       <c r="AI5">
-        <v>0.414937759336099</v>
+        <v>0.414651002073255</v>
       </c>
       <c r="AJ5">
-        <v>0.121023513139695</v>
+        <v>0.120939875604699</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">

</xml_diff>